<commit_message>
atualizacao dos documentos da casa
</commit_message>
<xml_diff>
--- a/Império Business Daily  (2).xlsx
+++ b/Império Business Daily  (2).xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="67">
   <si>
     <t>1ª SEMANA (Sprint Levantamento de Requisitos)</t>
   </si>
@@ -156,6 +156,36 @@
   </si>
   <si>
     <t xml:space="preserve"> Continuar o projeto no tinkercad</t>
+  </si>
+  <si>
+    <t>Atualizar o trello</t>
+  </si>
+  <si>
+    <t>Iniciou a montagem da casa com esp 32</t>
+  </si>
+  <si>
+    <t>montagem da casa com esp 32</t>
+  </si>
+  <si>
+    <t>Monitorou o trabalho da equipe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Monitorou o trabalho de equipe </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Atualizar o trello, Daily Scrum, estudar para a apresentacao </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Daily scrum, atualizar o trello, documentacao, e apresentacao </t>
+  </si>
+  <si>
+    <t>montagem da casa e do codigo com esp 32</t>
+  </si>
+  <si>
+    <t>monstagem da casa e do codigo com esp 32, daily scrum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Monitorou o trabalho de equipe, daily scrum, montar a documencao </t>
   </si>
   <si>
     <t>3ª SEMANA</t>
@@ -599,7 +629,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="91">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -752,41 +782,37 @@
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="16" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="center"/>
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="11" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="11" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="13" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="11" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="13" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="11" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="13" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="11" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" textRotation="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="11" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="11" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="13" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="11" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" textRotation="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="11" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="13" fillId="5" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="16" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="33" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
@@ -824,6 +850,9 @@
     </xf>
     <xf borderId="13" fillId="5" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="16" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="30" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
   </cellXfs>
@@ -1469,10 +1498,10 @@
       <c r="J15" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="K15" s="32" t="s">
+      <c r="K15" s="64" t="s">
         <v>10</v>
       </c>
-      <c r="L15" s="64" t="s">
+      <c r="L15" s="61" t="s">
         <v>10</v>
       </c>
       <c r="M15" s="65" t="s">
@@ -1501,137 +1530,197 @@
       <c r="C16" s="60">
         <v>45805.0</v>
       </c>
-      <c r="D16" s="64" t="s">
+      <c r="D16" s="68" t="s">
         <v>37</v>
       </c>
-      <c r="E16" s="64" t="s">
+      <c r="E16" s="68" t="s">
         <v>38</v>
       </c>
-      <c r="F16" s="64" t="s">
+      <c r="F16" s="61" t="s">
         <v>39</v>
       </c>
       <c r="G16" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="H16" s="64" t="s">
+      <c r="H16" s="68" t="s">
         <v>41</v>
       </c>
-      <c r="I16" s="64" t="s">
+      <c r="I16" s="61" t="s">
         <v>39</v>
       </c>
-      <c r="J16" s="36" t="s">
+      <c r="J16" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="K16" s="35" t="s">
+      <c r="K16" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="L16" s="35" t="s">
+      <c r="L16" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="M16" s="68" t="s">
+      <c r="M16" s="66" t="s">
         <v>22</v>
       </c>
-      <c r="N16" s="69" t="s">
+      <c r="N16" s="65" t="s">
         <v>22</v>
       </c>
-      <c r="O16" s="70" t="s">
+      <c r="O16" s="69" t="s">
         <v>22</v>
       </c>
-      <c r="P16" s="68" t="s">
+      <c r="P16" s="66" t="s">
         <v>42</v>
       </c>
-      <c r="Q16" s="68" t="s">
+      <c r="Q16" s="66" t="s">
         <v>43</v>
       </c>
-      <c r="R16" s="68" t="s">
+      <c r="R16" s="66" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="17" ht="14.25" customHeight="1">
-      <c r="B17" s="71" t="s">
-        <v>9</v>
+    <row r="17">
+      <c r="B17" s="70" t="s">
+        <v>23</v>
       </c>
       <c r="C17" s="60">
-        <v>45807.0</v>
-      </c>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="20"/>
-      <c r="H17" s="17"/>
-      <c r="I17" s="17"/>
-      <c r="J17" s="20"/>
-      <c r="K17" s="17"/>
-      <c r="L17" s="17"/>
-      <c r="M17" s="72"/>
-      <c r="N17" s="69"/>
-      <c r="O17" s="73"/>
-      <c r="P17" s="73"/>
-      <c r="Q17" s="73"/>
-      <c r="R17" s="73"/>
-    </row>
-    <row r="18" ht="14.25" customHeight="1">
-      <c r="B18" s="74" t="s">
-        <v>11</v>
+        <v>45819.0</v>
+      </c>
+      <c r="D17" s="68" t="s">
+        <v>33</v>
+      </c>
+      <c r="E17" s="32" t="s">
+        <v>44</v>
+      </c>
+      <c r="F17" s="64" t="s">
+        <v>39</v>
+      </c>
+      <c r="G17" s="62" t="s">
+        <v>45</v>
+      </c>
+      <c r="H17" s="61" t="s">
+        <v>46</v>
+      </c>
+      <c r="I17" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="J17" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="K17" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="L17" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="M17" s="71" t="s">
+        <v>45</v>
+      </c>
+      <c r="N17" s="72" t="s">
+        <v>46</v>
+      </c>
+      <c r="O17" s="65" t="s">
+        <v>39</v>
+      </c>
+      <c r="P17" s="65" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q17" s="66" t="s">
+        <v>48</v>
+      </c>
+      <c r="R17" s="65" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="B18" s="73" t="s">
+        <v>30</v>
       </c>
       <c r="C18" s="60">
-        <v>45807.0</v>
-      </c>
-      <c r="D18" s="17"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="17"/>
-      <c r="G18" s="18"/>
-      <c r="H18" s="19"/>
-      <c r="I18" s="19"/>
-      <c r="J18" s="75"/>
-      <c r="K18" s="17"/>
-      <c r="L18" s="17"/>
-      <c r="M18" s="72"/>
-      <c r="N18" s="58"/>
-      <c r="O18" s="58"/>
-      <c r="P18" s="58"/>
-      <c r="Q18" s="58"/>
-      <c r="R18" s="58"/>
+        <v>45819.0</v>
+      </c>
+      <c r="D18" s="68" t="s">
+        <v>49</v>
+      </c>
+      <c r="E18" s="68" t="s">
+        <v>50</v>
+      </c>
+      <c r="F18" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="G18" s="62" t="s">
+        <v>51</v>
+      </c>
+      <c r="H18" s="61" t="s">
+        <v>52</v>
+      </c>
+      <c r="I18" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="J18" s="62" t="s">
+        <v>21</v>
+      </c>
+      <c r="K18" s="61" t="s">
+        <v>21</v>
+      </c>
+      <c r="L18" s="64" t="s">
+        <v>21</v>
+      </c>
+      <c r="M18" s="71" t="s">
+        <v>51</v>
+      </c>
+      <c r="N18" s="66" t="s">
+        <v>52</v>
+      </c>
+      <c r="O18" s="69" t="s">
+        <v>39</v>
+      </c>
+      <c r="P18" s="66" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q18" s="66" t="s">
+        <v>53</v>
+      </c>
+      <c r="R18" s="65" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="19" ht="14.25" customHeight="1">
-      <c r="B19" s="76"/>
-      <c r="C19" s="77"/>
-      <c r="D19" s="78"/>
-      <c r="E19" s="78"/>
-      <c r="F19" s="78"/>
-      <c r="G19" s="79"/>
-      <c r="H19" s="78"/>
-      <c r="I19" s="78"/>
-      <c r="J19" s="80"/>
-      <c r="K19" s="81"/>
-      <c r="L19" s="81"/>
-      <c r="M19" s="82"/>
-      <c r="N19" s="82"/>
-      <c r="O19" s="82"/>
-      <c r="P19" s="82"/>
-      <c r="Q19" s="82"/>
-      <c r="R19" s="82"/>
+      <c r="B19" s="74"/>
+      <c r="C19" s="75"/>
+      <c r="D19" s="76"/>
+      <c r="E19" s="76"/>
+      <c r="F19" s="76"/>
+      <c r="G19" s="77"/>
+      <c r="H19" s="76"/>
+      <c r="I19" s="76"/>
+      <c r="J19" s="78"/>
+      <c r="K19" s="79"/>
+      <c r="L19" s="79"/>
+      <c r="M19" s="80"/>
+      <c r="N19" s="80"/>
+      <c r="O19" s="80"/>
+      <c r="P19" s="80"/>
+      <c r="Q19" s="80"/>
+      <c r="R19" s="80"/>
     </row>
     <row r="20" ht="14.25" customHeight="1"/>
     <row r="21" ht="14.25" customHeight="1"/>
     <row r="22" ht="14.25" customHeight="1"/>
     <row r="23" ht="14.25" customHeight="1">
       <c r="B23" s="47" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="C23" s="48"/>
-      <c r="D23" s="83" t="s">
-        <v>45</v>
+      <c r="D23" s="81" t="s">
+        <v>55</v>
       </c>
       <c r="E23" s="50"/>
       <c r="F23" s="51"/>
-      <c r="G23" s="84" t="s">
-        <v>46</v>
+      <c r="G23" s="82" t="s">
+        <v>56</v>
       </c>
       <c r="H23" s="50"/>
       <c r="I23" s="51"/>
-      <c r="J23" s="84" t="s">
-        <v>47</v>
+      <c r="J23" s="82" t="s">
+        <v>57</v>
       </c>
       <c r="K23" s="50"/>
       <c r="L23" s="51"/>
@@ -1663,7 +1752,7 @@
       <c r="K24" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="L24" s="85" t="s">
+      <c r="L24" s="83" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1678,13 +1767,13 @@
       <c r="I25" s="19"/>
       <c r="J25" s="20"/>
       <c r="K25" s="17"/>
-      <c r="L25" s="86"/>
+      <c r="L25" s="84"/>
     </row>
     <row r="26" ht="14.25" customHeight="1">
-      <c r="B26" s="87" t="s">
-        <v>48</v>
-      </c>
-      <c r="C26" s="88">
+      <c r="B26" s="85" t="s">
+        <v>58</v>
+      </c>
+      <c r="C26" s="86">
         <v>45509.0</v>
       </c>
       <c r="D26" s="19"/>
@@ -1695,13 +1784,13 @@
       <c r="I26" s="19"/>
       <c r="J26" s="20"/>
       <c r="K26" s="17"/>
-      <c r="L26" s="86"/>
+      <c r="L26" s="84"/>
     </row>
     <row r="27" ht="14.25" customHeight="1">
       <c r="B27" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="C27" s="88">
+        <v>59</v>
+      </c>
+      <c r="C27" s="86">
         <v>45510.0</v>
       </c>
       <c r="D27" s="17"/>
@@ -1712,13 +1801,13 @@
       <c r="I27" s="17"/>
       <c r="J27" s="20"/>
       <c r="K27" s="17"/>
-      <c r="L27" s="86"/>
+      <c r="L27" s="84"/>
     </row>
     <row r="28" ht="14.25" customHeight="1">
-      <c r="B28" s="89" t="s">
-        <v>50</v>
-      </c>
-      <c r="C28" s="88">
+      <c r="B28" s="87" t="s">
+        <v>60</v>
+      </c>
+      <c r="C28" s="86">
         <v>45511.0</v>
       </c>
       <c r="D28" s="17"/>
@@ -1729,13 +1818,13 @@
       <c r="I28" s="17"/>
       <c r="J28" s="20"/>
       <c r="K28" s="17"/>
-      <c r="L28" s="86"/>
+      <c r="L28" s="84"/>
     </row>
     <row r="29" ht="14.25" customHeight="1">
-      <c r="B29" s="90" t="s">
-        <v>51</v>
-      </c>
-      <c r="C29" s="88">
+      <c r="B29" s="88" t="s">
+        <v>61</v>
+      </c>
+      <c r="C29" s="86">
         <v>45512.0</v>
       </c>
       <c r="D29" s="17"/>
@@ -1744,47 +1833,47 @@
       <c r="G29" s="18"/>
       <c r="H29" s="19"/>
       <c r="I29" s="19"/>
-      <c r="J29" s="75"/>
+      <c r="J29" s="89"/>
       <c r="K29" s="17"/>
-      <c r="L29" s="86"/>
+      <c r="L29" s="84"/>
     </row>
     <row r="30" ht="14.25" customHeight="1">
-      <c r="B30" s="76" t="s">
-        <v>52</v>
-      </c>
-      <c r="C30" s="77">
+      <c r="B30" s="74" t="s">
+        <v>62</v>
+      </c>
+      <c r="C30" s="75">
         <v>45513.0</v>
       </c>
-      <c r="D30" s="78"/>
-      <c r="E30" s="78"/>
-      <c r="F30" s="78"/>
-      <c r="G30" s="79"/>
-      <c r="H30" s="78"/>
-      <c r="I30" s="78"/>
-      <c r="J30" s="80"/>
-      <c r="K30" s="81"/>
-      <c r="L30" s="91"/>
+      <c r="D30" s="76"/>
+      <c r="E30" s="76"/>
+      <c r="F30" s="76"/>
+      <c r="G30" s="77"/>
+      <c r="H30" s="76"/>
+      <c r="I30" s="76"/>
+      <c r="J30" s="78"/>
+      <c r="K30" s="79"/>
+      <c r="L30" s="90"/>
     </row>
     <row r="31" ht="14.25" customHeight="1"/>
     <row r="32" ht="14.25" customHeight="1"/>
     <row r="33" ht="14.25" customHeight="1"/>
     <row r="34" ht="14.25" customHeight="1">
       <c r="B34" s="47" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="C34" s="48"/>
-      <c r="D34" s="83" t="s">
-        <v>45</v>
+      <c r="D34" s="81" t="s">
+        <v>55</v>
       </c>
       <c r="E34" s="50"/>
       <c r="F34" s="51"/>
-      <c r="G34" s="84" t="s">
-        <v>46</v>
+      <c r="G34" s="82" t="s">
+        <v>56</v>
       </c>
       <c r="H34" s="50"/>
       <c r="I34" s="51"/>
-      <c r="J34" s="84" t="s">
-        <v>47</v>
+      <c r="J34" s="82" t="s">
+        <v>57</v>
       </c>
       <c r="K34" s="50"/>
       <c r="L34" s="51"/>
@@ -1816,7 +1905,7 @@
       <c r="K35" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="L35" s="85" t="s">
+      <c r="L35" s="83" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1831,13 +1920,13 @@
       <c r="I36" s="19"/>
       <c r="J36" s="20"/>
       <c r="K36" s="17"/>
-      <c r="L36" s="86"/>
+      <c r="L36" s="84"/>
     </row>
     <row r="37" ht="14.25" customHeight="1">
-      <c r="B37" s="87" t="s">
-        <v>48</v>
-      </c>
-      <c r="C37" s="88">
+      <c r="B37" s="85" t="s">
+        <v>58</v>
+      </c>
+      <c r="C37" s="86">
         <v>45516.0</v>
       </c>
       <c r="D37" s="19"/>
@@ -1848,13 +1937,13 @@
       <c r="I37" s="19"/>
       <c r="J37" s="20"/>
       <c r="K37" s="17"/>
-      <c r="L37" s="86"/>
+      <c r="L37" s="84"/>
     </row>
     <row r="38" ht="14.25" customHeight="1">
       <c r="B38" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="C38" s="88">
+        <v>59</v>
+      </c>
+      <c r="C38" s="86">
         <v>45517.0</v>
       </c>
       <c r="D38" s="17"/>
@@ -1865,13 +1954,13 @@
       <c r="I38" s="17"/>
       <c r="J38" s="20"/>
       <c r="K38" s="17"/>
-      <c r="L38" s="86"/>
+      <c r="L38" s="84"/>
     </row>
     <row r="39" ht="14.25" customHeight="1">
-      <c r="B39" s="89" t="s">
-        <v>50</v>
-      </c>
-      <c r="C39" s="88">
+      <c r="B39" s="87" t="s">
+        <v>60</v>
+      </c>
+      <c r="C39" s="86">
         <v>45518.0</v>
       </c>
       <c r="D39" s="17"/>
@@ -1882,13 +1971,13 @@
       <c r="I39" s="17"/>
       <c r="J39" s="20"/>
       <c r="K39" s="17"/>
-      <c r="L39" s="86"/>
+      <c r="L39" s="84"/>
     </row>
     <row r="40" ht="14.25" customHeight="1">
-      <c r="B40" s="90" t="s">
-        <v>51</v>
-      </c>
-      <c r="C40" s="88">
+      <c r="B40" s="88" t="s">
+        <v>61</v>
+      </c>
+      <c r="C40" s="86">
         <v>45519.0</v>
       </c>
       <c r="D40" s="17"/>
@@ -1897,47 +1986,47 @@
       <c r="G40" s="18"/>
       <c r="H40" s="19"/>
       <c r="I40" s="19"/>
-      <c r="J40" s="75"/>
+      <c r="J40" s="89"/>
       <c r="K40" s="17"/>
-      <c r="L40" s="86"/>
+      <c r="L40" s="84"/>
     </row>
     <row r="41" ht="14.25" customHeight="1">
-      <c r="B41" s="76" t="s">
-        <v>52</v>
-      </c>
-      <c r="C41" s="77">
+      <c r="B41" s="74" t="s">
+        <v>62</v>
+      </c>
+      <c r="C41" s="75">
         <v>45520.0</v>
       </c>
-      <c r="D41" s="78"/>
-      <c r="E41" s="78"/>
-      <c r="F41" s="78"/>
-      <c r="G41" s="79"/>
-      <c r="H41" s="78"/>
-      <c r="I41" s="78"/>
-      <c r="J41" s="80"/>
-      <c r="K41" s="81"/>
-      <c r="L41" s="91"/>
+      <c r="D41" s="76"/>
+      <c r="E41" s="76"/>
+      <c r="F41" s="76"/>
+      <c r="G41" s="77"/>
+      <c r="H41" s="76"/>
+      <c r="I41" s="76"/>
+      <c r="J41" s="78"/>
+      <c r="K41" s="79"/>
+      <c r="L41" s="90"/>
     </row>
     <row r="42" ht="14.25" customHeight="1"/>
     <row r="43" ht="14.25" customHeight="1"/>
     <row r="44" ht="14.25" customHeight="1"/>
     <row r="45" ht="14.25" customHeight="1">
       <c r="B45" s="47" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="C45" s="48"/>
-      <c r="D45" s="83" t="s">
-        <v>45</v>
+      <c r="D45" s="81" t="s">
+        <v>55</v>
       </c>
       <c r="E45" s="50"/>
       <c r="F45" s="51"/>
-      <c r="G45" s="84" t="s">
-        <v>46</v>
+      <c r="G45" s="82" t="s">
+        <v>56</v>
       </c>
       <c r="H45" s="50"/>
       <c r="I45" s="51"/>
-      <c r="J45" s="84" t="s">
-        <v>47</v>
+      <c r="J45" s="82" t="s">
+        <v>57</v>
       </c>
       <c r="K45" s="50"/>
       <c r="L45" s="51"/>
@@ -1969,7 +2058,7 @@
       <c r="K46" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="L46" s="85" t="s">
+      <c r="L46" s="83" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1984,13 +2073,13 @@
       <c r="I47" s="19"/>
       <c r="J47" s="20"/>
       <c r="K47" s="17"/>
-      <c r="L47" s="86"/>
+      <c r="L47" s="84"/>
     </row>
     <row r="48" ht="14.25" customHeight="1">
-      <c r="B48" s="87" t="s">
-        <v>48</v>
-      </c>
-      <c r="C48" s="88">
+      <c r="B48" s="85" t="s">
+        <v>58</v>
+      </c>
+      <c r="C48" s="86">
         <v>45523.0</v>
       </c>
       <c r="D48" s="19"/>
@@ -2001,13 +2090,13 @@
       <c r="I48" s="19"/>
       <c r="J48" s="20"/>
       <c r="K48" s="17"/>
-      <c r="L48" s="86"/>
+      <c r="L48" s="84"/>
     </row>
     <row r="49" ht="14.25" customHeight="1">
       <c r="B49" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="C49" s="88">
+        <v>59</v>
+      </c>
+      <c r="C49" s="86">
         <v>45524.0</v>
       </c>
       <c r="D49" s="17"/>
@@ -2018,13 +2107,13 @@
       <c r="I49" s="17"/>
       <c r="J49" s="20"/>
       <c r="K49" s="17"/>
-      <c r="L49" s="86"/>
+      <c r="L49" s="84"/>
     </row>
     <row r="50" ht="14.25" customHeight="1">
-      <c r="B50" s="89" t="s">
-        <v>50</v>
-      </c>
-      <c r="C50" s="88">
+      <c r="B50" s="87" t="s">
+        <v>60</v>
+      </c>
+      <c r="C50" s="86">
         <v>45525.0</v>
       </c>
       <c r="D50" s="17"/>
@@ -2035,13 +2124,13 @@
       <c r="I50" s="17"/>
       <c r="J50" s="20"/>
       <c r="K50" s="17"/>
-      <c r="L50" s="86"/>
+      <c r="L50" s="84"/>
     </row>
     <row r="51" ht="14.25" customHeight="1">
-      <c r="B51" s="90" t="s">
-        <v>51</v>
-      </c>
-      <c r="C51" s="88">
+      <c r="B51" s="88" t="s">
+        <v>61</v>
+      </c>
+      <c r="C51" s="86">
         <v>45526.0</v>
       </c>
       <c r="D51" s="17"/>
@@ -2050,47 +2139,47 @@
       <c r="G51" s="18"/>
       <c r="H51" s="19"/>
       <c r="I51" s="19"/>
-      <c r="J51" s="75"/>
+      <c r="J51" s="89"/>
       <c r="K51" s="17"/>
-      <c r="L51" s="86"/>
+      <c r="L51" s="84"/>
     </row>
     <row r="52" ht="14.25" customHeight="1">
-      <c r="B52" s="76" t="s">
-        <v>52</v>
-      </c>
-      <c r="C52" s="77">
+      <c r="B52" s="74" t="s">
+        <v>62</v>
+      </c>
+      <c r="C52" s="75">
         <v>45527.0</v>
       </c>
-      <c r="D52" s="78"/>
-      <c r="E52" s="78"/>
-      <c r="F52" s="78"/>
-      <c r="G52" s="79"/>
-      <c r="H52" s="78"/>
-      <c r="I52" s="78"/>
-      <c r="J52" s="80"/>
-      <c r="K52" s="81"/>
-      <c r="L52" s="91"/>
+      <c r="D52" s="76"/>
+      <c r="E52" s="76"/>
+      <c r="F52" s="76"/>
+      <c r="G52" s="77"/>
+      <c r="H52" s="76"/>
+      <c r="I52" s="76"/>
+      <c r="J52" s="78"/>
+      <c r="K52" s="79"/>
+      <c r="L52" s="90"/>
     </row>
     <row r="53" ht="14.25" customHeight="1"/>
     <row r="54" ht="14.25" customHeight="1"/>
     <row r="55" ht="14.25" customHeight="1"/>
     <row r="56" ht="14.25" customHeight="1">
       <c r="B56" s="47" t="s">
+        <v>65</v>
+      </c>
+      <c r="C56" s="48"/>
+      <c r="D56" s="81" t="s">
         <v>55</v>
-      </c>
-      <c r="C56" s="48"/>
-      <c r="D56" s="83" t="s">
-        <v>45</v>
       </c>
       <c r="E56" s="50"/>
       <c r="F56" s="51"/>
-      <c r="G56" s="84" t="s">
-        <v>46</v>
+      <c r="G56" s="82" t="s">
+        <v>56</v>
       </c>
       <c r="H56" s="50"/>
       <c r="I56" s="51"/>
-      <c r="J56" s="84" t="s">
-        <v>47</v>
+      <c r="J56" s="82" t="s">
+        <v>57</v>
       </c>
       <c r="K56" s="50"/>
       <c r="L56" s="51"/>
@@ -2122,7 +2211,7 @@
       <c r="K57" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="L57" s="85" t="s">
+      <c r="L57" s="83" t="s">
         <v>8</v>
       </c>
     </row>
@@ -2137,13 +2226,13 @@
       <c r="I58" s="19"/>
       <c r="J58" s="20"/>
       <c r="K58" s="17"/>
-      <c r="L58" s="86"/>
+      <c r="L58" s="84"/>
     </row>
     <row r="59" ht="14.25" customHeight="1">
-      <c r="B59" s="87" t="s">
-        <v>48</v>
-      </c>
-      <c r="C59" s="88">
+      <c r="B59" s="85" t="s">
+        <v>58</v>
+      </c>
+      <c r="C59" s="86">
         <v>45530.0</v>
       </c>
       <c r="D59" s="19"/>
@@ -2154,13 +2243,13 @@
       <c r="I59" s="19"/>
       <c r="J59" s="20"/>
       <c r="K59" s="17"/>
-      <c r="L59" s="86"/>
+      <c r="L59" s="84"/>
     </row>
     <row r="60" ht="14.25" customHeight="1">
       <c r="B60" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="C60" s="88">
+        <v>59</v>
+      </c>
+      <c r="C60" s="86">
         <v>45531.0</v>
       </c>
       <c r="D60" s="17"/>
@@ -2171,13 +2260,13 @@
       <c r="I60" s="17"/>
       <c r="J60" s="20"/>
       <c r="K60" s="17"/>
-      <c r="L60" s="86"/>
+      <c r="L60" s="84"/>
     </row>
     <row r="61" ht="14.25" customHeight="1">
-      <c r="B61" s="89" t="s">
-        <v>50</v>
-      </c>
-      <c r="C61" s="88">
+      <c r="B61" s="87" t="s">
+        <v>60</v>
+      </c>
+      <c r="C61" s="86">
         <v>45532.0</v>
       </c>
       <c r="D61" s="17"/>
@@ -2188,13 +2277,13 @@
       <c r="I61" s="17"/>
       <c r="J61" s="20"/>
       <c r="K61" s="17"/>
-      <c r="L61" s="86"/>
+      <c r="L61" s="84"/>
     </row>
     <row r="62" ht="14.25" customHeight="1">
-      <c r="B62" s="90" t="s">
-        <v>51</v>
-      </c>
-      <c r="C62" s="88">
+      <c r="B62" s="88" t="s">
+        <v>61</v>
+      </c>
+      <c r="C62" s="86">
         <v>45533.0</v>
       </c>
       <c r="D62" s="17"/>
@@ -2203,47 +2292,47 @@
       <c r="G62" s="18"/>
       <c r="H62" s="19"/>
       <c r="I62" s="19"/>
-      <c r="J62" s="75"/>
+      <c r="J62" s="89"/>
       <c r="K62" s="17"/>
-      <c r="L62" s="86"/>
+      <c r="L62" s="84"/>
     </row>
     <row r="63" ht="14.25" customHeight="1">
-      <c r="B63" s="76" t="s">
-        <v>52</v>
-      </c>
-      <c r="C63" s="77">
+      <c r="B63" s="74" t="s">
+        <v>62</v>
+      </c>
+      <c r="C63" s="75">
         <v>45534.0</v>
       </c>
-      <c r="D63" s="78"/>
-      <c r="E63" s="78"/>
-      <c r="F63" s="78"/>
-      <c r="G63" s="79"/>
-      <c r="H63" s="78"/>
-      <c r="I63" s="78"/>
-      <c r="J63" s="80"/>
-      <c r="K63" s="81"/>
-      <c r="L63" s="91"/>
+      <c r="D63" s="76"/>
+      <c r="E63" s="76"/>
+      <c r="F63" s="76"/>
+      <c r="G63" s="77"/>
+      <c r="H63" s="76"/>
+      <c r="I63" s="76"/>
+      <c r="J63" s="78"/>
+      <c r="K63" s="79"/>
+      <c r="L63" s="90"/>
     </row>
     <row r="64" ht="14.25" customHeight="1"/>
     <row r="65" ht="14.25" customHeight="1"/>
     <row r="66" ht="14.25" customHeight="1"/>
     <row r="67" ht="14.25" customHeight="1">
       <c r="B67" s="47" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="C67" s="48"/>
-      <c r="D67" s="83" t="s">
-        <v>45</v>
+      <c r="D67" s="81" t="s">
+        <v>55</v>
       </c>
       <c r="E67" s="50"/>
       <c r="F67" s="51"/>
-      <c r="G67" s="84" t="s">
-        <v>46</v>
+      <c r="G67" s="82" t="s">
+        <v>56</v>
       </c>
       <c r="H67" s="50"/>
       <c r="I67" s="51"/>
-      <c r="J67" s="84" t="s">
-        <v>47</v>
+      <c r="J67" s="82" t="s">
+        <v>57</v>
       </c>
       <c r="K67" s="50"/>
       <c r="L67" s="51"/>
@@ -2275,7 +2364,7 @@
       <c r="K68" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="L68" s="85" t="s">
+      <c r="L68" s="83" t="s">
         <v>8</v>
       </c>
     </row>
@@ -2290,13 +2379,13 @@
       <c r="I69" s="19"/>
       <c r="J69" s="20"/>
       <c r="K69" s="17"/>
-      <c r="L69" s="86"/>
+      <c r="L69" s="84"/>
     </row>
     <row r="70" ht="14.25" customHeight="1">
-      <c r="B70" s="87" t="s">
-        <v>48</v>
-      </c>
-      <c r="C70" s="88">
+      <c r="B70" s="85" t="s">
+        <v>58</v>
+      </c>
+      <c r="C70" s="86">
         <v>45537.0</v>
       </c>
       <c r="D70" s="19"/>
@@ -2307,13 +2396,13 @@
       <c r="I70" s="19"/>
       <c r="J70" s="20"/>
       <c r="K70" s="17"/>
-      <c r="L70" s="86"/>
+      <c r="L70" s="84"/>
     </row>
     <row r="71" ht="14.25" customHeight="1">
       <c r="B71" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="C71" s="88">
+        <v>59</v>
+      </c>
+      <c r="C71" s="86">
         <v>45538.0</v>
       </c>
       <c r="D71" s="17"/>
@@ -2324,13 +2413,13 @@
       <c r="I71" s="17"/>
       <c r="J71" s="20"/>
       <c r="K71" s="17"/>
-      <c r="L71" s="86"/>
+      <c r="L71" s="84"/>
     </row>
     <row r="72" ht="14.25" customHeight="1">
-      <c r="B72" s="89" t="s">
-        <v>50</v>
-      </c>
-      <c r="C72" s="88">
+      <c r="B72" s="87" t="s">
+        <v>60</v>
+      </c>
+      <c r="C72" s="86">
         <v>45539.0</v>
       </c>
       <c r="D72" s="17"/>
@@ -2341,13 +2430,13 @@
       <c r="I72" s="17"/>
       <c r="J72" s="20"/>
       <c r="K72" s="17"/>
-      <c r="L72" s="86"/>
+      <c r="L72" s="84"/>
     </row>
     <row r="73" ht="14.25" customHeight="1">
-      <c r="B73" s="90" t="s">
-        <v>51</v>
-      </c>
-      <c r="C73" s="88">
+      <c r="B73" s="88" t="s">
+        <v>61</v>
+      </c>
+      <c r="C73" s="86">
         <v>45540.0</v>
       </c>
       <c r="D73" s="17"/>
@@ -2356,26 +2445,26 @@
       <c r="G73" s="18"/>
       <c r="H73" s="19"/>
       <c r="I73" s="19"/>
-      <c r="J73" s="75"/>
+      <c r="J73" s="89"/>
       <c r="K73" s="17"/>
-      <c r="L73" s="86"/>
+      <c r="L73" s="84"/>
     </row>
     <row r="74" ht="14.25" customHeight="1">
-      <c r="B74" s="76" t="s">
-        <v>52</v>
-      </c>
-      <c r="C74" s="77">
+      <c r="B74" s="74" t="s">
+        <v>62</v>
+      </c>
+      <c r="C74" s="75">
         <v>45541.0</v>
       </c>
-      <c r="D74" s="78"/>
-      <c r="E74" s="78"/>
-      <c r="F74" s="78"/>
-      <c r="G74" s="79"/>
-      <c r="H74" s="78"/>
-      <c r="I74" s="78"/>
-      <c r="J74" s="80"/>
-      <c r="K74" s="81"/>
-      <c r="L74" s="91"/>
+      <c r="D74" s="76"/>
+      <c r="E74" s="76"/>
+      <c r="F74" s="76"/>
+      <c r="G74" s="77"/>
+      <c r="H74" s="76"/>
+      <c r="I74" s="76"/>
+      <c r="J74" s="78"/>
+      <c r="K74" s="79"/>
+      <c r="L74" s="90"/>
     </row>
     <row r="75" ht="14.25" customHeight="1"/>
     <row r="76" ht="14.25" customHeight="1"/>

</xml_diff>